<commit_message>
Added more R code including a tree
more data and images
</commit_message>
<xml_diff>
--- a/data/Employees - just qs.xlsx
+++ b/data/Employees - just qs.xlsx
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>frn_adminid</t>
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>SamOpinion</t>
   </si>
   <si>
     <t>NoTravel</t>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>NoSamHater</t>
+  </si>
+  <si>
+    <t>SamOpinion</t>
   </si>
   <si>
     <t>LightSamHater</t>
@@ -527,155 +527,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ88"/>
+  <dimension ref="A1:AY99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U67" sqref="U67"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
       <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
-        <v>21</v>
-      </c>
       <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="V1" t="s">
-        <v>27</v>
-      </c>
       <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" t="s">
-        <v>33</v>
-      </c>
       <c r="AB1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC1" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" t="s">
-        <v>39</v>
-      </c>
       <c r="AG1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>42</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>43</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" t="s">
-        <v>45</v>
-      </c>
       <c r="AL1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" t="s">
         <v>47</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>48</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>49</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" t="s">
-        <v>51</v>
-      </c>
       <c r="AQ1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR1" t="s">
         <v>53</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>54</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>55</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>56</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>57</v>
       </c>
       <c r="AV1" t="s">
         <v>58</v>
@@ -690,165 +688,162 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AF2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AG2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AI2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AJ2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AK2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AL2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AM2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AN2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AO2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AP2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AQ2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AR2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AS2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AT2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AU2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="AV2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="AW2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="AX2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="AY2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>241</v>
       </c>
@@ -1002,11 +997,8 @@
       <c r="AY3">
         <v>0</v>
       </c>
-      <c r="AZ3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>144</v>
       </c>
@@ -1160,11 +1152,8 @@
       <c r="AY4">
         <v>0</v>
       </c>
-      <c r="AZ4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>46</v>
       </c>
@@ -1318,11 +1307,8 @@
       <c r="AY5">
         <v>1</v>
       </c>
-      <c r="AZ5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>162</v>
       </c>
@@ -1476,11 +1462,8 @@
       <c r="AY6">
         <v>0</v>
       </c>
-      <c r="AZ6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>209</v>
       </c>
@@ -1634,11 +1617,8 @@
       <c r="AY7">
         <v>0</v>
       </c>
-      <c r="AZ7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>258</v>
       </c>
@@ -1792,11 +1772,8 @@
       <c r="AY8">
         <v>0</v>
       </c>
-      <c r="AZ8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1950,11 +1927,8 @@
       <c r="AY9">
         <v>0</v>
       </c>
-      <c r="AZ9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>59</v>
       </c>
@@ -2108,11 +2082,8 @@
       <c r="AY10">
         <v>0</v>
       </c>
-      <c r="AZ10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>245</v>
       </c>
@@ -2266,11 +2237,8 @@
       <c r="AY11">
         <v>0</v>
       </c>
-      <c r="AZ11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>161</v>
       </c>
@@ -2424,11 +2392,8 @@
       <c r="AY12">
         <v>0</v>
       </c>
-      <c r="AZ12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>87</v>
       </c>
@@ -2582,11 +2547,8 @@
       <c r="AY13">
         <v>1</v>
       </c>
-      <c r="AZ13">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>105</v>
       </c>
@@ -2740,11 +2702,8 @@
       <c r="AY14">
         <v>0</v>
       </c>
-      <c r="AZ14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>296</v>
       </c>
@@ -2898,11 +2857,8 @@
       <c r="AY15">
         <v>0</v>
       </c>
-      <c r="AZ15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>58</v>
       </c>
@@ -3056,11 +3012,8 @@
       <c r="AY16">
         <v>0</v>
       </c>
-      <c r="AZ16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>146</v>
       </c>
@@ -3214,11 +3167,8 @@
       <c r="AY17">
         <v>1</v>
       </c>
-      <c r="AZ17">
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>219</v>
       </c>
@@ -3372,11 +3322,8 @@
       <c r="AY18">
         <v>0</v>
       </c>
-      <c r="AZ18">
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>299</v>
       </c>
@@ -3530,11 +3477,8 @@
       <c r="AY19">
         <v>0</v>
       </c>
-      <c r="AZ19">
-        <v>0</v>
-      </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>282</v>
       </c>
@@ -3688,11 +3632,8 @@
       <c r="AY20">
         <v>0</v>
       </c>
-      <c r="AZ20">
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>223</v>
       </c>
@@ -3846,11 +3787,8 @@
       <c r="AY21">
         <v>0</v>
       </c>
-      <c r="AZ21">
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>211</v>
       </c>
@@ -4004,11 +3942,8 @@
       <c r="AY22">
         <v>0</v>
       </c>
-      <c r="AZ22">
-        <v>0</v>
-      </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>210</v>
       </c>
@@ -4162,11 +4097,8 @@
       <c r="AY23">
         <v>0</v>
       </c>
-      <c r="AZ23">
-        <v>0</v>
-      </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>320</v>
       </c>
@@ -4320,11 +4252,8 @@
       <c r="AY24">
         <v>0</v>
       </c>
-      <c r="AZ24">
-        <v>0</v>
-      </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>222</v>
       </c>
@@ -4478,11 +4407,8 @@
       <c r="AY25">
         <v>0</v>
       </c>
-      <c r="AZ25">
-        <v>0</v>
-      </c>
     </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>233</v>
       </c>
@@ -4636,11 +4562,8 @@
       <c r="AY26">
         <v>0</v>
       </c>
-      <c r="AZ26">
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>109</v>
       </c>
@@ -4794,11 +4717,8 @@
       <c r="AY27">
         <v>0</v>
       </c>
-      <c r="AZ27">
-        <v>0</v>
-      </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -4952,11 +4872,8 @@
       <c r="AY28">
         <v>1</v>
       </c>
-      <c r="AZ28">
-        <v>0</v>
-      </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>284</v>
       </c>
@@ -5110,11 +5027,8 @@
       <c r="AY29">
         <v>1</v>
       </c>
-      <c r="AZ29">
-        <v>0</v>
-      </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>117</v>
       </c>
@@ -5268,11 +5182,8 @@
       <c r="AY30">
         <v>0</v>
       </c>
-      <c r="AZ30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>57</v>
       </c>
@@ -5426,11 +5337,8 @@
       <c r="AY31">
         <v>0</v>
       </c>
-      <c r="AZ31">
-        <v>0</v>
-      </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -5584,11 +5492,8 @@
       <c r="AY32">
         <v>0</v>
       </c>
-      <c r="AZ32">
-        <v>0</v>
-      </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>301</v>
       </c>
@@ -5742,11 +5647,8 @@
       <c r="AY33">
         <v>0</v>
       </c>
-      <c r="AZ33">
-        <v>0</v>
-      </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>215</v>
       </c>
@@ -5900,11 +5802,8 @@
       <c r="AY34">
         <v>0</v>
       </c>
-      <c r="AZ34">
-        <v>0</v>
-      </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>206</v>
       </c>
@@ -6058,11 +5957,8 @@
       <c r="AY35">
         <v>1</v>
       </c>
-      <c r="AZ35">
-        <v>0</v>
-      </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>261</v>
       </c>
@@ -6216,11 +6112,8 @@
       <c r="AY36">
         <v>0</v>
       </c>
-      <c r="AZ36">
-        <v>0</v>
-      </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>199</v>
       </c>
@@ -6374,11 +6267,8 @@
       <c r="AY37">
         <v>0</v>
       </c>
-      <c r="AZ37">
-        <v>0</v>
-      </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>107</v>
       </c>
@@ -6532,11 +6422,8 @@
       <c r="AY38">
         <v>0</v>
       </c>
-      <c r="AZ38">
-        <v>0</v>
-      </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>195</v>
       </c>
@@ -6690,11 +6577,8 @@
       <c r="AY39">
         <v>0</v>
       </c>
-      <c r="AZ39">
-        <v>0</v>
-      </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>281</v>
       </c>
@@ -6848,11 +6732,8 @@
       <c r="AY40">
         <v>0</v>
       </c>
-      <c r="AZ40">
-        <v>0</v>
-      </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>329</v>
       </c>
@@ -7006,11 +6887,8 @@
       <c r="AY41">
         <v>0</v>
       </c>
-      <c r="AZ41">
-        <v>0</v>
-      </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>333</v>
       </c>
@@ -7164,11 +7042,8 @@
       <c r="AY42">
         <v>0</v>
       </c>
-      <c r="AZ42">
-        <v>0</v>
-      </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>341</v>
       </c>
@@ -7322,11 +7197,8 @@
       <c r="AY43">
         <v>0</v>
       </c>
-      <c r="AZ43">
-        <v>0</v>
-      </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>256</v>
       </c>
@@ -7480,11 +7352,8 @@
       <c r="AY44">
         <v>1</v>
       </c>
-      <c r="AZ44">
-        <v>0</v>
-      </c>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>251</v>
       </c>
@@ -7638,11 +7507,8 @@
       <c r="AY45">
         <v>0</v>
       </c>
-      <c r="AZ45">
-        <v>0</v>
-      </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>231</v>
       </c>
@@ -7796,11 +7662,8 @@
       <c r="AY46">
         <v>0</v>
       </c>
-      <c r="AZ46">
-        <v>0</v>
-      </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>76</v>
       </c>
@@ -7954,11 +7817,8 @@
       <c r="AY47">
         <v>0</v>
       </c>
-      <c r="AZ47">
-        <v>0</v>
-      </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>277</v>
       </c>
@@ -8112,11 +7972,8 @@
       <c r="AY48">
         <v>0</v>
       </c>
-      <c r="AZ48">
-        <v>0</v>
-      </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>273</v>
       </c>
@@ -8270,11 +8127,8 @@
       <c r="AY49">
         <v>0</v>
       </c>
-      <c r="AZ49">
-        <v>0</v>
-      </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>259</v>
       </c>
@@ -8428,11 +8282,8 @@
       <c r="AY50">
         <v>0</v>
       </c>
-      <c r="AZ50">
-        <v>0</v>
-      </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>39</v>
       </c>
@@ -8586,11 +8437,8 @@
       <c r="AY51">
         <v>0</v>
       </c>
-      <c r="AZ51">
-        <v>0</v>
-      </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>31</v>
       </c>
@@ -8744,11 +8592,8 @@
       <c r="AY52">
         <v>0</v>
       </c>
-      <c r="AZ52">
-        <v>0</v>
-      </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>325</v>
       </c>
@@ -8902,11 +8747,8 @@
       <c r="AY53">
         <v>0</v>
       </c>
-      <c r="AZ53">
-        <v>0</v>
-      </c>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>330</v>
       </c>
@@ -9060,11 +8902,8 @@
       <c r="AY54">
         <v>0</v>
       </c>
-      <c r="AZ54">
-        <v>0</v>
-      </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>279</v>
       </c>
@@ -9218,11 +9057,8 @@
       <c r="AY55">
         <v>0</v>
       </c>
-      <c r="AZ55">
-        <v>0</v>
-      </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>248</v>
       </c>
@@ -9376,11 +9212,8 @@
       <c r="AY56">
         <v>0</v>
       </c>
-      <c r="AZ56">
-        <v>0</v>
-      </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>303</v>
       </c>
@@ -9534,11 +9367,8 @@
       <c r="AY57">
         <v>0</v>
       </c>
-      <c r="AZ57">
-        <v>0</v>
-      </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>286</v>
       </c>
@@ -9692,11 +9522,8 @@
       <c r="AY58">
         <v>0</v>
       </c>
-      <c r="AZ58">
-        <v>0</v>
-      </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>278</v>
       </c>
@@ -9850,11 +9677,8 @@
       <c r="AY59">
         <v>0</v>
       </c>
-      <c r="AZ59">
-        <v>0</v>
-      </c>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>96</v>
       </c>
@@ -10008,11 +9832,8 @@
       <c r="AY60">
         <v>1</v>
       </c>
-      <c r="AZ60">
-        <v>0</v>
-      </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>67</v>
       </c>
@@ -10166,11 +9987,8 @@
       <c r="AY61">
         <v>0</v>
       </c>
-      <c r="AZ61">
-        <v>0</v>
-      </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>285</v>
       </c>
@@ -10324,11 +10142,8 @@
       <c r="AY62">
         <v>0</v>
       </c>
-      <c r="AZ62">
-        <v>0</v>
-      </c>
     </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>122</v>
       </c>
@@ -10482,11 +10297,8 @@
       <c r="AY63">
         <v>1</v>
       </c>
-      <c r="AZ63">
-        <v>0</v>
-      </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>275</v>
       </c>
@@ -10640,11 +10452,8 @@
       <c r="AY64">
         <v>0</v>
       </c>
-      <c r="AZ64">
-        <v>0</v>
-      </c>
     </row>
-    <row r="65" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>300</v>
       </c>
@@ -10798,11 +10607,8 @@
       <c r="AY65">
         <v>0</v>
       </c>
-      <c r="AZ65">
-        <v>0</v>
-      </c>
     </row>
-    <row r="66" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>137</v>
       </c>
@@ -10956,11 +10762,8 @@
       <c r="AY66">
         <v>0</v>
       </c>
-      <c r="AZ66">
-        <v>0</v>
-      </c>
     </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>302</v>
       </c>
@@ -11114,11 +10917,8 @@
       <c r="AY67">
         <v>1</v>
       </c>
-      <c r="AZ67">
-        <v>0</v>
-      </c>
     </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>155</v>
       </c>
@@ -11272,11 +11072,8 @@
       <c r="AY68">
         <v>0</v>
       </c>
-      <c r="AZ68">
-        <v>0</v>
-      </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>236</v>
       </c>
@@ -11430,11 +11227,8 @@
       <c r="AY69">
         <v>0</v>
       </c>
-      <c r="AZ69">
-        <v>0</v>
-      </c>
     </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>79</v>
       </c>
@@ -11588,11 +11382,8 @@
       <c r="AY70">
         <v>1</v>
       </c>
-      <c r="AZ70">
-        <v>0</v>
-      </c>
     </row>
-    <row r="71" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>106</v>
       </c>
@@ -11746,11 +11537,8 @@
       <c r="AY71">
         <v>0</v>
       </c>
-      <c r="AZ71">
-        <v>0</v>
-      </c>
     </row>
-    <row r="72" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>154</v>
       </c>
@@ -11904,11 +11692,8 @@
       <c r="AY72">
         <v>0</v>
       </c>
-      <c r="AZ72">
-        <v>0</v>
-      </c>
     </row>
-    <row r="73" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>264</v>
       </c>
@@ -12062,11 +11847,8 @@
       <c r="AY73">
         <v>1</v>
       </c>
-      <c r="AZ73">
-        <v>0</v>
-      </c>
     </row>
-    <row r="74" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>294</v>
       </c>
@@ -12220,11 +12002,8 @@
       <c r="AY74">
         <v>1</v>
       </c>
-      <c r="AZ74">
-        <v>0</v>
-      </c>
     </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>216</v>
       </c>
@@ -12378,11 +12157,8 @@
       <c r="AY75">
         <v>1</v>
       </c>
-      <c r="AZ75">
-        <v>0</v>
-      </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>321</v>
       </c>
@@ -12536,11 +12312,8 @@
       <c r="AY76">
         <v>0</v>
       </c>
-      <c r="AZ76">
-        <v>0</v>
-      </c>
     </row>
-    <row r="77" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>254</v>
       </c>
@@ -12694,11 +12467,8 @@
       <c r="AY77">
         <v>0</v>
       </c>
-      <c r="AZ77">
-        <v>0</v>
-      </c>
     </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>150</v>
       </c>
@@ -12852,11 +12622,8 @@
       <c r="AY78">
         <v>0</v>
       </c>
-      <c r="AZ78">
-        <v>0</v>
-      </c>
     </row>
-    <row r="79" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>324</v>
       </c>
@@ -13010,11 +12777,8 @@
       <c r="AY79">
         <v>0</v>
       </c>
-      <c r="AZ79">
-        <v>0</v>
-      </c>
     </row>
-    <row r="80" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>262</v>
       </c>
@@ -13168,11 +12932,8 @@
       <c r="AY80">
         <v>0</v>
       </c>
-      <c r="AZ80">
-        <v>0</v>
-      </c>
     </row>
-    <row r="81" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>287</v>
       </c>
@@ -13326,11 +13087,8 @@
       <c r="AY81">
         <v>0</v>
       </c>
-      <c r="AZ81">
-        <v>0</v>
-      </c>
     </row>
-    <row r="82" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>276</v>
       </c>
@@ -13484,11 +13242,8 @@
       <c r="AY82">
         <v>0</v>
       </c>
-      <c r="AZ82">
-        <v>0</v>
-      </c>
     </row>
-    <row r="83" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>335</v>
       </c>
@@ -13642,11 +13397,8 @@
       <c r="AY83">
         <v>0</v>
       </c>
-      <c r="AZ83">
-        <v>0</v>
-      </c>
     </row>
-    <row r="84" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>112</v>
       </c>
@@ -13800,11 +13552,8 @@
       <c r="AY84">
         <v>0</v>
       </c>
-      <c r="AZ84">
-        <v>0</v>
-      </c>
     </row>
-    <row r="85" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>21</v>
       </c>
@@ -13958,11 +13707,8 @@
       <c r="AY85">
         <v>0</v>
       </c>
-      <c r="AZ85">
-        <v>0</v>
-      </c>
     </row>
-    <row r="86" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1</v>
       </c>
@@ -14116,11 +13862,8 @@
       <c r="AY86">
         <v>0</v>
       </c>
-      <c r="AZ86">
-        <v>0</v>
-      </c>
     </row>
-    <row r="87" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>214</v>
       </c>
@@ -14274,11 +14017,8 @@
       <c r="AY87">
         <v>0</v>
       </c>
-      <c r="AZ87">
-        <v>0</v>
-      </c>
     </row>
-    <row r="88" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>197</v>
       </c>
@@ -14432,7 +14172,1676 @@
       <c r="AY88">
         <v>0</v>
       </c>
-      <c r="AZ88">
+    </row>
+    <row r="89" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+      <c r="S89">
+        <v>0</v>
+      </c>
+      <c r="T89">
+        <v>1</v>
+      </c>
+      <c r="U89">
+        <v>0</v>
+      </c>
+      <c r="V89">
+        <v>0</v>
+      </c>
+      <c r="W89">
+        <v>0</v>
+      </c>
+      <c r="X89">
+        <v>0</v>
+      </c>
+      <c r="Y89">
+        <v>0</v>
+      </c>
+      <c r="Z89">
+        <v>1</v>
+      </c>
+      <c r="AA89">
+        <v>0</v>
+      </c>
+      <c r="AB89">
+        <v>0</v>
+      </c>
+      <c r="AC89">
+        <v>0</v>
+      </c>
+      <c r="AD89">
+        <v>1</v>
+      </c>
+      <c r="AE89">
+        <v>0</v>
+      </c>
+      <c r="AF89">
+        <v>0</v>
+      </c>
+      <c r="AG89">
+        <v>0</v>
+      </c>
+      <c r="AH89">
+        <v>0</v>
+      </c>
+      <c r="AI89">
+        <v>0</v>
+      </c>
+      <c r="AJ89">
+        <v>1</v>
+      </c>
+      <c r="AK89">
+        <v>0</v>
+      </c>
+      <c r="AL89">
+        <v>0</v>
+      </c>
+      <c r="AM89">
+        <v>1</v>
+      </c>
+      <c r="AN89">
+        <v>0</v>
+      </c>
+      <c r="AO89">
+        <v>0</v>
+      </c>
+      <c r="AP89">
+        <v>0</v>
+      </c>
+      <c r="AQ89">
+        <v>0</v>
+      </c>
+      <c r="AR89">
+        <v>0</v>
+      </c>
+      <c r="AS89">
+        <v>1</v>
+      </c>
+      <c r="AT89">
+        <v>0</v>
+      </c>
+      <c r="AU89">
+        <v>1</v>
+      </c>
+      <c r="AV89">
+        <v>0</v>
+      </c>
+      <c r="AW89">
+        <v>0</v>
+      </c>
+      <c r="AX89">
+        <v>0</v>
+      </c>
+      <c r="AY89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90">
+        <v>1</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+      <c r="S90">
+        <v>0</v>
+      </c>
+      <c r="T90">
+        <v>1</v>
+      </c>
+      <c r="U90">
+        <v>0</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>0</v>
+      </c>
+      <c r="X90">
+        <v>1</v>
+      </c>
+      <c r="Y90">
+        <v>0</v>
+      </c>
+      <c r="Z90">
+        <v>0</v>
+      </c>
+      <c r="AA90">
+        <v>0</v>
+      </c>
+      <c r="AB90">
+        <v>0</v>
+      </c>
+      <c r="AC90">
+        <v>1</v>
+      </c>
+      <c r="AD90">
+        <v>0</v>
+      </c>
+      <c r="AE90">
+        <v>0</v>
+      </c>
+      <c r="AF90">
+        <v>0</v>
+      </c>
+      <c r="AG90">
+        <v>0</v>
+      </c>
+      <c r="AH90">
+        <v>0</v>
+      </c>
+      <c r="AI90">
+        <v>1</v>
+      </c>
+      <c r="AJ90">
+        <v>0</v>
+      </c>
+      <c r="AK90">
+        <v>0</v>
+      </c>
+      <c r="AL90">
+        <v>1</v>
+      </c>
+      <c r="AM90">
+        <v>0</v>
+      </c>
+      <c r="AN90">
+        <v>0</v>
+      </c>
+      <c r="AO90">
+        <v>0</v>
+      </c>
+      <c r="AP90">
+        <v>0</v>
+      </c>
+      <c r="AQ90">
+        <v>0</v>
+      </c>
+      <c r="AR90">
+        <v>0</v>
+      </c>
+      <c r="AS90">
+        <v>1</v>
+      </c>
+      <c r="AT90">
+        <v>0</v>
+      </c>
+      <c r="AU90">
+        <v>0</v>
+      </c>
+      <c r="AV90">
+        <v>0</v>
+      </c>
+      <c r="AW90">
+        <v>1</v>
+      </c>
+      <c r="AX90">
+        <v>0</v>
+      </c>
+      <c r="AY90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+      <c r="N91">
+        <v>0</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="R91">
+        <v>0</v>
+      </c>
+      <c r="S91">
+        <v>0</v>
+      </c>
+      <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="U91">
+        <v>1</v>
+      </c>
+      <c r="V91">
+        <v>1</v>
+      </c>
+      <c r="W91">
+        <v>0</v>
+      </c>
+      <c r="X91">
+        <v>0</v>
+      </c>
+      <c r="Y91">
+        <v>0</v>
+      </c>
+      <c r="Z91">
+        <v>0</v>
+      </c>
+      <c r="AA91">
+        <v>0</v>
+      </c>
+      <c r="AB91">
+        <v>1</v>
+      </c>
+      <c r="AC91">
+        <v>0</v>
+      </c>
+      <c r="AD91">
+        <v>0</v>
+      </c>
+      <c r="AE91">
+        <v>0</v>
+      </c>
+      <c r="AF91">
+        <v>0</v>
+      </c>
+      <c r="AG91">
+        <v>0</v>
+      </c>
+      <c r="AH91">
+        <v>0</v>
+      </c>
+      <c r="AI91">
+        <v>0</v>
+      </c>
+      <c r="AJ91">
+        <v>1</v>
+      </c>
+      <c r="AK91">
+        <v>0</v>
+      </c>
+      <c r="AL91">
+        <v>0</v>
+      </c>
+      <c r="AM91">
+        <v>0</v>
+      </c>
+      <c r="AN91">
+        <v>0</v>
+      </c>
+      <c r="AO91">
+        <v>1</v>
+      </c>
+      <c r="AP91">
+        <v>0</v>
+      </c>
+      <c r="AQ91">
+        <v>0</v>
+      </c>
+      <c r="AR91">
+        <v>0</v>
+      </c>
+      <c r="AS91">
+        <v>1</v>
+      </c>
+      <c r="AT91">
+        <v>0</v>
+      </c>
+      <c r="AU91">
+        <v>0</v>
+      </c>
+      <c r="AV91">
+        <v>1</v>
+      </c>
+      <c r="AW91">
+        <v>0</v>
+      </c>
+      <c r="AX91">
+        <v>0</v>
+      </c>
+      <c r="AY91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+      <c r="S92">
+        <v>0</v>
+      </c>
+      <c r="T92">
+        <v>1</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <v>1</v>
+      </c>
+      <c r="W92">
+        <v>0</v>
+      </c>
+      <c r="X92">
+        <v>0</v>
+      </c>
+      <c r="Y92">
+        <v>0</v>
+      </c>
+      <c r="Z92">
+        <v>0</v>
+      </c>
+      <c r="AA92">
+        <v>0</v>
+      </c>
+      <c r="AB92">
+        <v>1</v>
+      </c>
+      <c r="AC92">
+        <v>0</v>
+      </c>
+      <c r="AD92">
+        <v>0</v>
+      </c>
+      <c r="AE92">
+        <v>0</v>
+      </c>
+      <c r="AF92">
+        <v>0</v>
+      </c>
+      <c r="AG92">
+        <v>1</v>
+      </c>
+      <c r="AH92">
+        <v>0</v>
+      </c>
+      <c r="AI92">
+        <v>0</v>
+      </c>
+      <c r="AJ92">
+        <v>0</v>
+      </c>
+      <c r="AK92">
+        <v>1</v>
+      </c>
+      <c r="AL92">
+        <v>0</v>
+      </c>
+      <c r="AM92">
+        <v>0</v>
+      </c>
+      <c r="AN92">
+        <v>0</v>
+      </c>
+      <c r="AO92">
+        <v>0</v>
+      </c>
+      <c r="AP92">
+        <v>0</v>
+      </c>
+      <c r="AQ92">
+        <v>1</v>
+      </c>
+      <c r="AR92">
+        <v>0</v>
+      </c>
+      <c r="AS92">
+        <v>0</v>
+      </c>
+      <c r="AT92">
+        <v>0</v>
+      </c>
+      <c r="AU92">
+        <v>1</v>
+      </c>
+      <c r="AV92">
+        <v>0</v>
+      </c>
+      <c r="AW92">
+        <v>0</v>
+      </c>
+      <c r="AX92">
+        <v>0</v>
+      </c>
+      <c r="AY92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <v>0</v>
+      </c>
+      <c r="S93">
+        <v>0</v>
+      </c>
+      <c r="T93">
+        <v>1</v>
+      </c>
+      <c r="U93">
+        <v>0</v>
+      </c>
+      <c r="V93">
+        <v>1</v>
+      </c>
+      <c r="W93">
+        <v>0</v>
+      </c>
+      <c r="X93">
+        <v>0</v>
+      </c>
+      <c r="Y93">
+        <v>0</v>
+      </c>
+      <c r="Z93">
+        <v>0</v>
+      </c>
+      <c r="AA93">
+        <v>0</v>
+      </c>
+      <c r="AB93">
+        <v>0</v>
+      </c>
+      <c r="AC93">
+        <v>0</v>
+      </c>
+      <c r="AD93">
+        <v>1</v>
+      </c>
+      <c r="AE93">
+        <v>0</v>
+      </c>
+      <c r="AF93">
+        <v>0</v>
+      </c>
+      <c r="AG93">
+        <v>0</v>
+      </c>
+      <c r="AH93">
+        <v>0</v>
+      </c>
+      <c r="AI93">
+        <v>0</v>
+      </c>
+      <c r="AJ93">
+        <v>1</v>
+      </c>
+      <c r="AK93">
+        <v>0</v>
+      </c>
+      <c r="AL93">
+        <v>0</v>
+      </c>
+      <c r="AM93">
+        <v>0</v>
+      </c>
+      <c r="AN93">
+        <v>1</v>
+      </c>
+      <c r="AO93">
+        <v>0</v>
+      </c>
+      <c r="AP93">
+        <v>0</v>
+      </c>
+      <c r="AQ93">
+        <v>1</v>
+      </c>
+      <c r="AR93">
+        <v>0</v>
+      </c>
+      <c r="AS93">
+        <v>0</v>
+      </c>
+      <c r="AT93">
+        <v>0</v>
+      </c>
+      <c r="AU93">
+        <v>0</v>
+      </c>
+      <c r="AV93">
+        <v>0</v>
+      </c>
+      <c r="AW93">
+        <v>0</v>
+      </c>
+      <c r="AX93">
+        <v>1</v>
+      </c>
+      <c r="AY93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>1</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
+      <c r="R94">
+        <v>0</v>
+      </c>
+      <c r="S94">
+        <v>0</v>
+      </c>
+      <c r="T94">
+        <v>1</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>1</v>
+      </c>
+      <c r="X94">
+        <v>0</v>
+      </c>
+      <c r="Y94">
+        <v>0</v>
+      </c>
+      <c r="Z94">
+        <v>0</v>
+      </c>
+      <c r="AA94">
+        <v>0</v>
+      </c>
+      <c r="AB94">
+        <v>1</v>
+      </c>
+      <c r="AC94">
+        <v>0</v>
+      </c>
+      <c r="AD94">
+        <v>0</v>
+      </c>
+      <c r="AE94">
+        <v>0</v>
+      </c>
+      <c r="AF94">
+        <v>0</v>
+      </c>
+      <c r="AG94">
+        <v>0</v>
+      </c>
+      <c r="AH94">
+        <v>0</v>
+      </c>
+      <c r="AI94">
+        <v>1</v>
+      </c>
+      <c r="AJ94">
+        <v>0</v>
+      </c>
+      <c r="AK94">
+        <v>0</v>
+      </c>
+      <c r="AL94">
+        <v>0</v>
+      </c>
+      <c r="AM94">
+        <v>0</v>
+      </c>
+      <c r="AN94">
+        <v>1</v>
+      </c>
+      <c r="AO94">
+        <v>0</v>
+      </c>
+      <c r="AP94">
+        <v>0</v>
+      </c>
+      <c r="AQ94">
+        <v>1</v>
+      </c>
+      <c r="AR94">
+        <v>0</v>
+      </c>
+      <c r="AS94">
+        <v>0</v>
+      </c>
+      <c r="AT94">
+        <v>0</v>
+      </c>
+      <c r="AU94">
+        <v>0</v>
+      </c>
+      <c r="AV94">
+        <v>0</v>
+      </c>
+      <c r="AW94">
+        <v>1</v>
+      </c>
+      <c r="AX94">
+        <v>0</v>
+      </c>
+      <c r="AY94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>1</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95">
+        <v>0</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
+      </c>
+      <c r="U95">
+        <v>0</v>
+      </c>
+      <c r="V95">
+        <v>1</v>
+      </c>
+      <c r="W95">
+        <v>0</v>
+      </c>
+      <c r="X95">
+        <v>0</v>
+      </c>
+      <c r="Y95">
+        <v>0</v>
+      </c>
+      <c r="Z95">
+        <v>0</v>
+      </c>
+      <c r="AA95">
+        <v>0</v>
+      </c>
+      <c r="AB95">
+        <v>0</v>
+      </c>
+      <c r="AC95">
+        <v>0</v>
+      </c>
+      <c r="AD95">
+        <v>0</v>
+      </c>
+      <c r="AE95">
+        <v>1</v>
+      </c>
+      <c r="AF95">
+        <v>0</v>
+      </c>
+      <c r="AG95">
+        <v>0</v>
+      </c>
+      <c r="AH95">
+        <v>0</v>
+      </c>
+      <c r="AI95">
+        <v>0</v>
+      </c>
+      <c r="AJ95">
+        <v>1</v>
+      </c>
+      <c r="AK95">
+        <v>1</v>
+      </c>
+      <c r="AL95">
+        <v>0</v>
+      </c>
+      <c r="AM95">
+        <v>0</v>
+      </c>
+      <c r="AN95">
+        <v>0</v>
+      </c>
+      <c r="AO95">
+        <v>0</v>
+      </c>
+      <c r="AP95">
+        <v>0</v>
+      </c>
+      <c r="AQ95">
+        <v>1</v>
+      </c>
+      <c r="AR95">
+        <v>0</v>
+      </c>
+      <c r="AS95">
+        <v>0</v>
+      </c>
+      <c r="AT95">
+        <v>0</v>
+      </c>
+      <c r="AU95">
+        <v>0</v>
+      </c>
+      <c r="AV95">
+        <v>1</v>
+      </c>
+      <c r="AW95">
+        <v>0</v>
+      </c>
+      <c r="AX95">
+        <v>0</v>
+      </c>
+      <c r="AY95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>1</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
+      </c>
+      <c r="W96">
+        <v>1</v>
+      </c>
+      <c r="X96">
+        <v>0</v>
+      </c>
+      <c r="Y96">
+        <v>0</v>
+      </c>
+      <c r="Z96">
+        <v>0</v>
+      </c>
+      <c r="AA96">
+        <v>0</v>
+      </c>
+      <c r="AB96">
+        <v>0</v>
+      </c>
+      <c r="AC96">
+        <v>0</v>
+      </c>
+      <c r="AD96">
+        <v>0</v>
+      </c>
+      <c r="AE96">
+        <v>1</v>
+      </c>
+      <c r="AF96">
+        <v>0</v>
+      </c>
+      <c r="AG96">
+        <v>0</v>
+      </c>
+      <c r="AH96">
+        <v>1</v>
+      </c>
+      <c r="AI96">
+        <v>0</v>
+      </c>
+      <c r="AJ96">
+        <v>0</v>
+      </c>
+      <c r="AK96">
+        <v>0</v>
+      </c>
+      <c r="AL96">
+        <v>0</v>
+      </c>
+      <c r="AM96">
+        <v>0</v>
+      </c>
+      <c r="AN96">
+        <v>0</v>
+      </c>
+      <c r="AO96">
+        <v>1</v>
+      </c>
+      <c r="AP96">
+        <v>0</v>
+      </c>
+      <c r="AQ96">
+        <v>0</v>
+      </c>
+      <c r="AR96">
+        <v>0</v>
+      </c>
+      <c r="AS96">
+        <v>1</v>
+      </c>
+      <c r="AT96">
+        <v>0</v>
+      </c>
+      <c r="AU96">
+        <v>0</v>
+      </c>
+      <c r="AV96">
+        <v>0</v>
+      </c>
+      <c r="AW96">
+        <v>0</v>
+      </c>
+      <c r="AX96">
+        <v>1</v>
+      </c>
+      <c r="AY96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
+      <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+      <c r="T97">
+        <v>1</v>
+      </c>
+      <c r="U97">
+        <v>0</v>
+      </c>
+      <c r="V97">
+        <v>0</v>
+      </c>
+      <c r="W97">
+        <v>0</v>
+      </c>
+      <c r="X97">
+        <v>1</v>
+      </c>
+      <c r="Y97">
+        <v>0</v>
+      </c>
+      <c r="Z97">
+        <v>0</v>
+      </c>
+      <c r="AA97">
+        <v>0</v>
+      </c>
+      <c r="AB97">
+        <v>0</v>
+      </c>
+      <c r="AC97">
+        <v>1</v>
+      </c>
+      <c r="AD97">
+        <v>0</v>
+      </c>
+      <c r="AE97">
+        <v>0</v>
+      </c>
+      <c r="AF97">
+        <v>0</v>
+      </c>
+      <c r="AG97">
+        <v>0</v>
+      </c>
+      <c r="AH97">
+        <v>0</v>
+      </c>
+      <c r="AI97">
+        <v>0</v>
+      </c>
+      <c r="AJ97">
+        <v>1</v>
+      </c>
+      <c r="AK97">
+        <v>0</v>
+      </c>
+      <c r="AL97">
+        <v>0</v>
+      </c>
+      <c r="AM97">
+        <v>1</v>
+      </c>
+      <c r="AN97">
+        <v>0</v>
+      </c>
+      <c r="AO97">
+        <v>0</v>
+      </c>
+      <c r="AP97">
+        <v>0</v>
+      </c>
+      <c r="AQ97">
+        <v>0</v>
+      </c>
+      <c r="AR97">
+        <v>0</v>
+      </c>
+      <c r="AS97">
+        <v>1</v>
+      </c>
+      <c r="AT97">
+        <v>0</v>
+      </c>
+      <c r="AU97">
+        <v>1</v>
+      </c>
+      <c r="AV97">
+        <v>0</v>
+      </c>
+      <c r="AW97">
+        <v>0</v>
+      </c>
+      <c r="AX97">
+        <v>0</v>
+      </c>
+      <c r="AY97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>1</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
+      <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+      <c r="T98">
+        <v>1</v>
+      </c>
+      <c r="U98">
+        <v>0</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>0</v>
+      </c>
+      <c r="X98">
+        <v>0</v>
+      </c>
+      <c r="Y98">
+        <v>1</v>
+      </c>
+      <c r="Z98">
+        <v>0</v>
+      </c>
+      <c r="AA98">
+        <v>0</v>
+      </c>
+      <c r="AB98">
+        <v>0</v>
+      </c>
+      <c r="AC98">
+        <v>0</v>
+      </c>
+      <c r="AD98">
+        <v>0</v>
+      </c>
+      <c r="AE98">
+        <v>1</v>
+      </c>
+      <c r="AF98">
+        <v>0</v>
+      </c>
+      <c r="AG98">
+        <v>0</v>
+      </c>
+      <c r="AH98">
+        <v>1</v>
+      </c>
+      <c r="AI98">
+        <v>0</v>
+      </c>
+      <c r="AJ98">
+        <v>0</v>
+      </c>
+      <c r="AK98">
+        <v>0</v>
+      </c>
+      <c r="AL98">
+        <v>0</v>
+      </c>
+      <c r="AM98">
+        <v>0</v>
+      </c>
+      <c r="AN98">
+        <v>1</v>
+      </c>
+      <c r="AO98">
+        <v>0</v>
+      </c>
+      <c r="AP98">
+        <v>0</v>
+      </c>
+      <c r="AQ98">
+        <v>1</v>
+      </c>
+      <c r="AR98">
+        <v>0</v>
+      </c>
+      <c r="AS98">
+        <v>0</v>
+      </c>
+      <c r="AT98">
+        <v>0</v>
+      </c>
+      <c r="AU98">
+        <v>0</v>
+      </c>
+      <c r="AV98">
+        <v>0</v>
+      </c>
+      <c r="AW98">
+        <v>1</v>
+      </c>
+      <c r="AX98">
+        <v>0</v>
+      </c>
+      <c r="AY98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>1</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>0</v>
+      </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+      <c r="T99">
+        <v>1</v>
+      </c>
+      <c r="U99">
+        <v>0</v>
+      </c>
+      <c r="V99">
+        <v>0</v>
+      </c>
+      <c r="W99">
+        <v>0</v>
+      </c>
+      <c r="X99">
+        <v>0</v>
+      </c>
+      <c r="Y99">
+        <v>0</v>
+      </c>
+      <c r="Z99">
+        <v>1</v>
+      </c>
+      <c r="AA99">
+        <v>0</v>
+      </c>
+      <c r="AB99">
+        <v>0</v>
+      </c>
+      <c r="AC99">
+        <v>0</v>
+      </c>
+      <c r="AD99">
+        <v>0</v>
+      </c>
+      <c r="AE99">
+        <v>1</v>
+      </c>
+      <c r="AF99">
+        <v>0</v>
+      </c>
+      <c r="AG99">
+        <v>0</v>
+      </c>
+      <c r="AH99">
+        <v>0</v>
+      </c>
+      <c r="AI99">
+        <v>1</v>
+      </c>
+      <c r="AJ99">
+        <v>0</v>
+      </c>
+      <c r="AK99">
+        <v>0</v>
+      </c>
+      <c r="AL99">
+        <v>1</v>
+      </c>
+      <c r="AM99">
+        <v>0</v>
+      </c>
+      <c r="AN99">
+        <v>0</v>
+      </c>
+      <c r="AO99">
+        <v>0</v>
+      </c>
+      <c r="AP99">
+        <v>0</v>
+      </c>
+      <c r="AQ99">
+        <v>1</v>
+      </c>
+      <c r="AR99">
+        <v>0</v>
+      </c>
+      <c r="AS99">
+        <v>0</v>
+      </c>
+      <c r="AT99">
+        <v>0</v>
+      </c>
+      <c r="AU99">
+        <v>0</v>
+      </c>
+      <c r="AV99">
+        <v>1</v>
+      </c>
+      <c r="AW99">
+        <v>0</v>
+      </c>
+      <c r="AX99">
+        <v>0</v>
+      </c>
+      <c r="AY99">
         <v>0</v>
       </c>
     </row>

</xml_diff>